<commit_message>
interface criada, ids guardadas
</commit_message>
<xml_diff>
--- a/id-class-function.xlsx
+++ b/id-class-function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aprendizado\site anime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C707CE-74A6-4EC8-A413-D1D45F96787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184271B9-6F94-4A80-831D-F44FCCCF7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="855" windowWidth="9975" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="855" windowWidth="7680" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>HTML</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>Função</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>id-section-bloco-menu</t>
+  </si>
+  <si>
+    <t>Menu superior fixo</t>
+  </si>
+  <si>
+    <t>id-article-body</t>
+  </si>
+  <si>
+    <t>representa o body, arquivo principal</t>
   </si>
 </sst>
 </file>
@@ -464,13 +479,13 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="G2:J10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
@@ -507,10 +522,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="7"/>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -519,10 +540,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>

</xml_diff>

<commit_message>
class e id referente ao menu adicionado
</commit_message>
<xml_diff>
--- a/id-class-function.xlsx
+++ b/id-class-function.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aprendizado\site anime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184271B9-6F94-4A80-831D-F44FCCCF7D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494F87C0-2605-42F7-B9A8-00CA9C3F0859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12585" yWindow="855" windowWidth="7680" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>HTML</t>
   </si>
@@ -58,6 +58,36 @@
   </si>
   <si>
     <t>representa o body, arquivo principal</t>
+  </si>
+  <si>
+    <t>id-div-container</t>
+  </si>
+  <si>
+    <t>container de tudo</t>
+  </si>
+  <si>
+    <t>class-img-logo</t>
+  </si>
+  <si>
+    <t>logotipo, generica</t>
+  </si>
+  <si>
+    <t>nav pai do ul e li</t>
+  </si>
+  <si>
+    <t>id-nav-pai-ul</t>
+  </si>
+  <si>
+    <t>class-li</t>
+  </si>
+  <si>
+    <t>filhos ul</t>
+  </si>
+  <si>
+    <t>id-ul-pai-li</t>
+  </si>
+  <si>
+    <t>controla a lista</t>
   </si>
 </sst>
 </file>
@@ -479,7 +509,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,10 +588,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -570,10 +606,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -582,10 +624,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -594,10 +642,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -606,10 +660,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>

</xml_diff>